<commit_message>
MainESPCAM made. So far it is functional for canny edge detection and angle calculation of found edge
</commit_message>
<xml_diff>
--- a/Project/findOptimalThresholdControlLogic.xlsx
+++ b/Project/findOptimalThresholdControlLogic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian Lykke\Documents\Skole\Aalborg Universitet\ESD5\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6459FD43-3D1A-4971-BE2E-CEF02F43C4BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605E4D46-083E-4A39-AF90-8C9CEB61CC0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{CC48EEEC-788B-40F3-9568-5026D52638E2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CC48EEEC-788B-40F3-9568-5026D52638E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -640,7 +640,7 @@
   <dimension ref="A1:II94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1424,7 +1424,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="10">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="F2" s="10">
         <f>ROUNDUP(D2/30,0)</f>
@@ -1455,7 +1455,7 @@
       </c>
       <c r="M2" s="10">
         <f>E2+1</f>
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="N2" s="10">
         <f>ROUNDUP(L2/30,0)</f>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="U2" s="10">
         <f>M2+1</f>
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="V2" s="10">
         <f>ROUNDUP(T2/30,0)</f>
@@ -1517,7 +1517,7 @@
       </c>
       <c r="AC2" s="10">
         <f>U2+1</f>
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="AD2" s="10">
         <f>ROUNDUP(AB2/30,0)</f>
@@ -1548,7 +1548,7 @@
       </c>
       <c r="AK2" s="10">
         <f>AC2+1</f>
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="AL2" s="10">
         <f>ROUNDUP(AJ2/30,0)</f>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="AS2" s="10">
         <f>AK2+1</f>
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="AT2" s="10">
         <f>ROUNDUP(AR2/30,0)</f>
@@ -1610,7 +1610,7 @@
       </c>
       <c r="BA2" s="10">
         <f>AS2+1</f>
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="BB2" s="10">
         <f>ROUNDUP(AZ2/30,0)</f>
@@ -1641,7 +1641,7 @@
       </c>
       <c r="BI2" s="10">
         <f>BA2+1</f>
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="BJ2" s="10">
         <f>ROUNDUP(BH2/30,0)</f>
@@ -1672,7 +1672,7 @@
       </c>
       <c r="BQ2" s="10">
         <f>BI2+1</f>
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="BR2" s="10">
         <f>ROUNDUP(BP2/30,0)</f>
@@ -1703,7 +1703,7 @@
       </c>
       <c r="BY2" s="10">
         <f>BQ2+1</f>
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="BZ2" s="10">
         <f>ROUNDUP(BX2/30,0)</f>
@@ -1734,7 +1734,7 @@
       </c>
       <c r="CG2" s="10">
         <f>BY2+1</f>
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="CH2" s="10">
         <f>ROUNDUP(CF2/30,0)</f>
@@ -1765,7 +1765,7 @@
       </c>
       <c r="CO2" s="10">
         <f>CG2+1</f>
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="CP2" s="10">
         <f>ROUNDUP(CN2/30,0)</f>
@@ -1796,7 +1796,7 @@
       </c>
       <c r="CW2" s="10">
         <f>CO2+1</f>
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="CX2" s="10">
         <f>ROUNDUP(CV2/30,0)</f>
@@ -1827,7 +1827,7 @@
       </c>
       <c r="DE2" s="10">
         <f>CW2+1</f>
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="DF2" s="10">
         <f>ROUNDUP(DD2/30,0)</f>
@@ -1858,7 +1858,7 @@
       </c>
       <c r="DM2" s="10">
         <f>DE2+1</f>
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="DN2" s="10">
         <f>ROUNDUP(DL2/30,0)</f>
@@ -1889,7 +1889,7 @@
       </c>
       <c r="DU2" s="10">
         <f>DM2+1</f>
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="DV2" s="10">
         <f>ROUNDUP(DT2/30,0)</f>
@@ -1920,7 +1920,7 @@
       </c>
       <c r="EC2" s="10">
         <f>DU2+1</f>
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="ED2" s="10">
         <f>ROUNDUP(EB2/30,0)</f>
@@ -1951,7 +1951,7 @@
       </c>
       <c r="EK2" s="10">
         <f>EC2+1</f>
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="EL2" s="10">
         <f>ROUNDUP(EJ2/30,0)</f>
@@ -1982,7 +1982,7 @@
       </c>
       <c r="ES2" s="10">
         <f>EK2+1</f>
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="ET2" s="10">
         <f>ROUNDUP(ER2/30,0)</f>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="FA2" s="10">
         <f>ES2+1</f>
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="FB2" s="10">
         <f>ROUNDUP(EZ2/30,0)</f>
@@ -2044,7 +2044,7 @@
       </c>
       <c r="FI2" s="10">
         <f>FA2+1</f>
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="FJ2" s="10">
         <f>ROUNDUP(FH2/30,0)</f>
@@ -2075,7 +2075,7 @@
       </c>
       <c r="FQ2" s="10">
         <f>FI2+1</f>
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="FR2" s="10">
         <f>ROUNDUP(FP2/30,0)</f>
@@ -2106,7 +2106,7 @@
       </c>
       <c r="FY2" s="10">
         <f>FQ2+1</f>
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="FZ2" s="10">
         <f>ROUNDUP(FX2/30,0)</f>
@@ -2137,7 +2137,7 @@
       </c>
       <c r="GG2" s="10">
         <f>FY2+1</f>
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="GH2" s="10">
         <f>ROUNDUP(GF2/30,0)</f>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="GO2" s="10">
         <f>GG2+1</f>
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="GP2" s="10">
         <f>ROUNDUP(GN2/30,0)</f>
@@ -2199,7 +2199,7 @@
       </c>
       <c r="GW2" s="10">
         <f>GO2+1</f>
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="GX2" s="10">
         <f>ROUNDUP(GV2/30,0)</f>
@@ -2230,7 +2230,7 @@
       </c>
       <c r="HE2" s="10">
         <f>GW2+1</f>
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="HF2" s="10">
         <f>ROUNDUP(HD2/30,0)</f>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="HM2" s="10">
         <f>HE2+1</f>
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="HN2" s="10">
         <f>ROUNDUP(HL2/30,0)</f>
@@ -2292,7 +2292,7 @@
       </c>
       <c r="HU2" s="10">
         <f>HM2+1</f>
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="HV2" s="10">
         <f>ROUNDUP(HT2/30,0)</f>
@@ -2323,7 +2323,7 @@
       </c>
       <c r="IC2" s="10">
         <f>HU2+1</f>
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="ID2" s="10">
         <f>ROUNDUP(IB2/30,0)</f>

</xml_diff>